<commit_message>
Update Personalizaciones ERP - CCG.xlsx
</commit_message>
<xml_diff>
--- a/Personalizaciones ERP - CCG.xlsx
+++ b/Personalizaciones ERP - CCG.xlsx
@@ -902,7 +902,7 @@
   <dimension ref="A1:D133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135"/>
+      <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2364,7 +2364,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" ht="10.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
         <v>4</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>107</v>
       </c>
       <c r="D105" s="16" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>